<commit_message>
SLC reg and sponsor plan
</commit_message>
<xml_diff>
--- a/assets/misc/2023/2023_Attendance.xlsx
+++ b/assets/misc/2023/2023_Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FDFF40-DCE7-4B10-B08B-35806D14653F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF8BEAC-1DE4-4220-BA2A-8F45BAAFD83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26790" yWindow="2040" windowWidth="23820" windowHeight="13710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1035" windowWidth="25815" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Event</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>SQL Saturday Denver 2023</t>
+  </si>
+  <si>
+    <t>Recordings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Saturday Boston 2023 </t>
+  </si>
+  <si>
+    <t>SQL Saturday Columbus</t>
+  </si>
+  <si>
+    <t>SQL Saturday SLC</t>
   </si>
 </sst>
 </file>
@@ -427,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +455,7 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -465,8 +477,11 @@
       <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -487,7 +502,7 @@
         <v>0.28813559322033899</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -511,7 +526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -532,7 +547,7 @@
         <v>0.26267281105990781</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -542,12 +557,18 @@
       <c r="C5" s="1">
         <v>45003</v>
       </c>
+      <c r="D5">
+        <v>236</v>
+      </c>
+      <c r="E5">
+        <v>106</v>
+      </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.55084745762711862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -557,12 +578,18 @@
       <c r="C6" s="1">
         <v>45017</v>
       </c>
+      <c r="E6">
+        <v>280</v>
+      </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -577,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -592,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -607,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -622,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -637,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -652,28 +679,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="F16" s="2">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
attendance and south island redirect
</commit_message>
<xml_diff>
--- a/assets/misc/2023/2023_Attendance.xlsx
+++ b/assets/misc/2023/2023_Attendance.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\way0u\Documents\git\sqlsatwebsite\assets\misc\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B5C53-09E0-4C45-87DC-EFB516D89558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECAA66C-E38B-42EC-AC00-C91ADC792BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23430" yWindow="0" windowWidth="20880" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Event</t>
   </si>
@@ -114,6 +103,9 @@
   </si>
   <si>
     <t>200 at last count on YT</t>
+  </si>
+  <si>
+    <t>SQL Saturday Los Angeles 2023</t>
   </si>
 </sst>
 </file>
@@ -454,20 +446,20 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -496,7 +488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -517,7 +509,7 @@
         <v>0.28813559322033899</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -541,7 +533,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -562,7 +554,7 @@
         <v>0.26267281105990781</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -583,7 +575,7 @@
         <v>0.55084745762711862</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -604,7 +596,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -631,7 +623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -655,7 +647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -679,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -689,9 +681,18 @@
       <c r="C10" s="1">
         <v>45066</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -701,12 +702,15 @@
       <c r="C11" s="1">
         <v>45080</v>
       </c>
+      <c r="E11">
+        <v>120</v>
+      </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -721,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -736,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -746,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -756,24 +760,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>1049</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45087</v>
+      </c>
+      <c r="D16">
+        <v>257</v>
+      </c>
+      <c r="E16">
+        <v>135</v>
+      </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+        <v>0.47470817120622566</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated old data from 2023
</commit_message>
<xml_diff>
--- a/assets/misc/2023/2023_Attendance.xlsx
+++ b/assets/misc/2023/2023_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ABBC9B-9C3E-46AA-AF6A-B3F1F5B33DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7054CA8-779E-42DB-A4CF-C275B3C1135F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26745" yWindow="300" windowWidth="21615" windowHeight="15015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="810" windowWidth="26070" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Event</t>
   </si>
@@ -496,7 +496,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>84</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:F25" si="0">IF(D2=0,0,+(D2-E2)/D2)</f>
+        <f t="shared" ref="F2:F26" si="0">IF(D2=0,0,+(D2-E2)/D2)</f>
         <v>0.28813559322033899</v>
       </c>
     </row>
@@ -1060,10 +1060,31 @@
         <v>0.60472972972972971</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>1057</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45241</v>
+      </c>
+      <c r="D26">
+        <v>331</v>
+      </c>
+      <c r="E26">
+        <v>266</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19637462235649547</v>
+      </c>
+    </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E27">
-        <f>SUM(E2:E25)</f>
-        <v>4060</v>
+        <f>SUM(E2:E26)</f>
+        <v>4326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>